<commit_message>
structured code for one season
</commit_message>
<xml_diff>
--- a/merged_data.xlsx
+++ b/merged_data.xlsx
@@ -556,211 +556,211 @@
     <t>17 Apr 1985</t>
   </si>
   <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>710</t>
-  </si>
-  <si>
-    <t>69</t>
-  </si>
-  <si>
-    <t>701</t>
-  </si>
-  <si>
-    <t>375</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>134</t>
+    <t>25</t>
+  </si>
+  <si>
+    <t>711</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>699</t>
+  </si>
+  <si>
+    <t>344</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>147</t>
   </si>
   <si>
     <t>940</t>
   </si>
   <si>
-    <t>93</t>
+    <t>94</t>
   </si>
   <si>
     <t>101</t>
   </si>
   <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>604</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>287</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>663</t>
+  </si>
+  <si>
+    <t>332</t>
+  </si>
+  <si>
+    <t>512</t>
+  </si>
+  <si>
+    <t>244</t>
+  </si>
+  <si>
+    <t>461</t>
+  </si>
+  <si>
+    <t>519</t>
+  </si>
+  <si>
+    <t>213</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>227</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>282</t>
+  </si>
+  <si>
+    <t>687</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>238</t>
+  </si>
+  <si>
+    <t>197</t>
+  </si>
+  <si>
+    <t>177</t>
+  </si>
+  <si>
+    <t>199=</t>
+  </si>
+  <si>
+    <t>307</t>
+  </si>
+  <si>
+    <t>281</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>568=</t>
+  </si>
+  <si>
+    <t>195</t>
+  </si>
+  <si>
+    <t>841</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>906</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>529</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>198</t>
+  </si>
+  <si>
+    <t>25 Aug 1981</t>
+  </si>
+  <si>
+    <t>05 Aug 1992</t>
+  </si>
+  <si>
+    <t>13 Feb 1986</t>
+  </si>
+  <si>
+    <t>25 Jul 1988</t>
+  </si>
+  <si>
+    <t>24 Dec 1988</t>
+  </si>
+  <si>
+    <t>15 Feb 1987</t>
+  </si>
+  <si>
+    <t>04 Jul 1993</t>
+  </si>
+  <si>
+    <t>07 May 1992</t>
+  </si>
+  <si>
+    <t>309</t>
+  </si>
+  <si>
+    <t>829</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>210</t>
+  </si>
+  <si>
+    <t>17=</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
     <t>48</t>
   </si>
   <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>253</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>287</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>602</t>
-  </si>
-  <si>
-    <t>336</t>
-  </si>
-  <si>
-    <t>512</t>
-  </si>
-  <si>
-    <t>242</t>
-  </si>
-  <si>
-    <t>467</t>
-  </si>
-  <si>
-    <t>524</t>
-  </si>
-  <si>
-    <t>211</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>204</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>281</t>
-  </si>
-  <si>
-    <t>679</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>77</t>
-  </si>
-  <si>
-    <t>124</t>
-  </si>
-  <si>
-    <t>73</t>
-  </si>
-  <si>
-    <t>237</t>
-  </si>
-  <si>
-    <t>196=</t>
-  </si>
-  <si>
-    <t>221</t>
-  </si>
-  <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>311</t>
-  </si>
-  <si>
-    <t>230</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>569=</t>
-  </si>
-  <si>
-    <t>195</t>
-  </si>
-  <si>
-    <t>837</t>
-  </si>
-  <si>
-    <t>114</t>
-  </si>
-  <si>
-    <t>905</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>530</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>199</t>
-  </si>
-  <si>
-    <t>25 Aug 1981</t>
-  </si>
-  <si>
-    <t>05 Aug 1992</t>
-  </si>
-  <si>
-    <t>13 Feb 1986</t>
-  </si>
-  <si>
-    <t>25 Jul 1988</t>
-  </si>
-  <si>
-    <t>24 Dec 1988</t>
-  </si>
-  <si>
-    <t>15 Feb 1987</t>
-  </si>
-  <si>
-    <t>04 Jul 1993</t>
-  </si>
-  <si>
-    <t>07 May 1992</t>
-  </si>
-  <si>
-    <t>320</t>
-  </si>
-  <si>
-    <t>833</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>218</t>
-  </si>
-  <si>
-    <t>18=</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>836</t>
+    <t>22</t>
+  </si>
+  <si>
+    <t>840</t>
   </si>
 </sst>
 </file>
@@ -1533,7 +1533,7 @@
         <v>184</v>
       </c>
       <c r="T8" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U8" t="s">
         <v>120</v>
@@ -1542,7 +1542,7 @@
         <v>174</v>
       </c>
       <c r="X8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:24">
@@ -1595,7 +1595,7 @@
         <v>184</v>
       </c>
       <c r="T9" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U9" t="s">
         <v>120</v>
@@ -1604,7 +1604,7 @@
         <v>174</v>
       </c>
       <c r="X9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10" spans="1:24">
@@ -1657,7 +1657,7 @@
         <v>184</v>
       </c>
       <c r="T10" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U10" t="s">
         <v>120</v>
@@ -1666,7 +1666,7 @@
         <v>174</v>
       </c>
       <c r="X10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:24">
@@ -1719,7 +1719,7 @@
         <v>184</v>
       </c>
       <c r="T11" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U11" t="s">
         <v>120</v>
@@ -1728,7 +1728,7 @@
         <v>174</v>
       </c>
       <c r="X11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="12" spans="1:24">
@@ -1781,7 +1781,7 @@
         <v>184</v>
       </c>
       <c r="T12" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U12" t="s">
         <v>120</v>
@@ -1790,7 +1790,7 @@
         <v>174</v>
       </c>
       <c r="X12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:24">
@@ -1843,7 +1843,7 @@
         <v>184</v>
       </c>
       <c r="T13" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U13" t="s">
         <v>120</v>
@@ -1852,7 +1852,7 @@
         <v>174</v>
       </c>
       <c r="X13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="14" spans="1:24">
@@ -1905,7 +1905,7 @@
         <v>184</v>
       </c>
       <c r="T14" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U14" t="s">
         <v>120</v>
@@ -1914,7 +1914,7 @@
         <v>174</v>
       </c>
       <c r="X14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15" spans="1:24">
@@ -1967,7 +1967,7 @@
         <v>184</v>
       </c>
       <c r="T15" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U15" t="s">
         <v>120</v>
@@ -1976,7 +1976,7 @@
         <v>174</v>
       </c>
       <c r="X15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="16" spans="1:24">
@@ -2029,7 +2029,7 @@
         <v>184</v>
       </c>
       <c r="T16" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U16" t="s">
         <v>120</v>
@@ -2038,7 +2038,7 @@
         <v>174</v>
       </c>
       <c r="X16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="17" spans="1:24">
@@ -2091,7 +2091,7 @@
         <v>184</v>
       </c>
       <c r="T17" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U17" t="s">
         <v>120</v>
@@ -2100,7 +2100,7 @@
         <v>174</v>
       </c>
       <c r="X17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="18" spans="1:24">
@@ -2153,7 +2153,7 @@
         <v>184</v>
       </c>
       <c r="T18" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U18" t="s">
         <v>120</v>
@@ -2162,7 +2162,7 @@
         <v>174</v>
       </c>
       <c r="X18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" spans="1:24">
@@ -2215,7 +2215,7 @@
         <v>184</v>
       </c>
       <c r="T19" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U19" t="s">
         <v>120</v>
@@ -2224,7 +2224,7 @@
         <v>174</v>
       </c>
       <c r="X19" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="20" spans="1:24">
@@ -2283,10 +2283,10 @@
         <v>121</v>
       </c>
       <c r="V20" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="X20" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21" spans="1:24">
@@ -2570,7 +2570,7 @@
         <v>186</v>
       </c>
       <c r="T27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="28" spans="1:24">
@@ -2620,7 +2620,7 @@
         <v>186</v>
       </c>
       <c r="T28" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="29" spans="1:24">
@@ -2805,19 +2805,19 @@
         <v>141</v>
       </c>
       <c r="T32" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="U32" t="s">
         <v>122</v>
       </c>
       <c r="V32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="W32" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="X32" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="33" spans="1:24">
@@ -2867,7 +2867,7 @@
         <v>142</v>
       </c>
       <c r="T33" t="s">
-        <v>198</v>
+        <v>214</v>
       </c>
       <c r="U33" t="s">
         <v>123</v>
@@ -2879,7 +2879,7 @@
         <v>186</v>
       </c>
       <c r="X33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="34" spans="1:24">
@@ -2929,7 +2929,7 @@
         <v>142</v>
       </c>
       <c r="T34" t="s">
-        <v>198</v>
+        <v>214</v>
       </c>
       <c r="U34" t="s">
         <v>123</v>
@@ -2941,7 +2941,7 @@
         <v>186</v>
       </c>
       <c r="X34" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="35" spans="1:24">
@@ -2991,7 +2991,7 @@
         <v>142</v>
       </c>
       <c r="T35" t="s">
-        <v>198</v>
+        <v>214</v>
       </c>
       <c r="U35" t="s">
         <v>123</v>
@@ -3003,7 +3003,7 @@
         <v>186</v>
       </c>
       <c r="X35" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="36" spans="1:24">
@@ -3053,7 +3053,7 @@
         <v>142</v>
       </c>
       <c r="T36" t="s">
-        <v>198</v>
+        <v>214</v>
       </c>
       <c r="U36" t="s">
         <v>123</v>
@@ -3065,7 +3065,7 @@
         <v>186</v>
       </c>
       <c r="X36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="37" spans="1:24">
@@ -3162,7 +3162,7 @@
         <v>186</v>
       </c>
       <c r="T38" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="39" spans="1:24">
@@ -3212,7 +3212,7 @@
         <v>186</v>
       </c>
       <c r="T39" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="40" spans="1:24">
@@ -3964,10 +3964,10 @@
         <v>125</v>
       </c>
       <c r="V55" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="X55" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="56" spans="1:24">
@@ -4510,10 +4510,10 @@
         <v>126</v>
       </c>
       <c r="V67" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="X67" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="68" spans="1:24">
@@ -4563,7 +4563,7 @@
         <v>154</v>
       </c>
       <c r="T68" t="s">
-        <v>222</v>
+        <v>180</v>
       </c>
       <c r="U68" t="s">
         <v>127</v>
@@ -4625,7 +4625,7 @@
         <v>154</v>
       </c>
       <c r="T69" t="s">
-        <v>222</v>
+        <v>180</v>
       </c>
       <c r="U69" t="s">
         <v>127</v>
@@ -4687,7 +4687,7 @@
         <v>154</v>
       </c>
       <c r="T70" t="s">
-        <v>222</v>
+        <v>180</v>
       </c>
       <c r="U70" t="s">
         <v>127</v>
@@ -4749,7 +4749,7 @@
         <v>154</v>
       </c>
       <c r="T71" t="s">
-        <v>222</v>
+        <v>180</v>
       </c>
       <c r="U71" t="s">
         <v>127</v>
@@ -5183,7 +5183,7 @@
         <v>197</v>
       </c>
       <c r="T81" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="82" spans="1:24">
@@ -5312,7 +5312,7 @@
         <v>198</v>
       </c>
       <c r="T84" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="85" spans="1:24">
@@ -5368,7 +5368,7 @@
         <v>169</v>
       </c>
       <c r="X85" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="86" spans="1:24">
@@ -5424,7 +5424,7 @@
         <v>169</v>
       </c>
       <c r="X86" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="87" spans="1:24">
@@ -5480,7 +5480,7 @@
         <v>169</v>
       </c>
       <c r="X87" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="88" spans="1:24">
@@ -5536,7 +5536,7 @@
         <v>169</v>
       </c>
       <c r="X88" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="89" spans="1:24">
@@ -5592,7 +5592,7 @@
         <v>169</v>
       </c>
       <c r="X89" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="90" spans="1:24">
@@ -5648,7 +5648,7 @@
         <v>169</v>
       </c>
       <c r="X90" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="91" spans="1:24">
@@ -5704,7 +5704,7 @@
         <v>169</v>
       </c>
       <c r="X91" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="92" spans="1:24">
@@ -5760,7 +5760,7 @@
         <v>169</v>
       </c>
       <c r="X92" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="93" spans="1:24">
@@ -5816,7 +5816,7 @@
         <v>169</v>
       </c>
       <c r="X93" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="94" spans="1:24">
@@ -5872,7 +5872,7 @@
         <v>169</v>
       </c>
       <c r="X94" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="95" spans="1:24">
@@ -5928,7 +5928,7 @@
         <v>169</v>
       </c>
       <c r="X95" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="96" spans="1:24">
@@ -5984,7 +5984,7 @@
         <v>169</v>
       </c>
       <c r="X96" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="97" spans="1:24">
@@ -6040,7 +6040,7 @@
         <v>169</v>
       </c>
       <c r="X97" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="98" spans="1:24">
@@ -6096,7 +6096,7 @@
         <v>169</v>
       </c>
       <c r="X98" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="99" spans="1:24">
@@ -6152,7 +6152,7 @@
         <v>169</v>
       </c>
       <c r="X99" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="100" spans="1:24">
@@ -6208,7 +6208,7 @@
         <v>169</v>
       </c>
       <c r="X100" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="101" spans="1:24">
@@ -6264,7 +6264,7 @@
         <v>197</v>
       </c>
       <c r="X101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="102" spans="1:24">
@@ -6487,7 +6487,7 @@
         <v>198</v>
       </c>
       <c r="T106" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="107" spans="1:24">
@@ -6662,7 +6662,7 @@
         <v>200</v>
       </c>
       <c r="T111" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="112" spans="1:24">
@@ -6709,7 +6709,7 @@
         <v>200</v>
       </c>
       <c r="T112" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="113" spans="1:24">
@@ -6756,7 +6756,7 @@
         <v>200</v>
       </c>
       <c r="T113" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="114" spans="1:24">
@@ -6803,7 +6803,7 @@
         <v>200</v>
       </c>
       <c r="T114" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="115" spans="1:24">
@@ -6853,7 +6853,7 @@
         <v>186</v>
       </c>
       <c r="T115" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="116" spans="1:24">
@@ -6903,7 +6903,7 @@
         <v>186</v>
       </c>
       <c r="T116" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="117" spans="1:24">
@@ -6953,7 +6953,7 @@
         <v>201</v>
       </c>
       <c r="T117" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="118" spans="1:24">
@@ -7003,7 +7003,7 @@
         <v>201</v>
       </c>
       <c r="T118" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="119" spans="1:24">
@@ -7050,7 +7050,7 @@
         <v>142</v>
       </c>
       <c r="T119" t="s">
-        <v>198</v>
+        <v>214</v>
       </c>
       <c r="U119" t="s">
         <v>123</v>
@@ -7062,7 +7062,7 @@
         <v>186</v>
       </c>
       <c r="X119" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="120" spans="1:24">
@@ -7109,7 +7109,7 @@
         <v>142</v>
       </c>
       <c r="T120" t="s">
-        <v>198</v>
+        <v>214</v>
       </c>
       <c r="U120" t="s">
         <v>123</v>
@@ -7121,7 +7121,7 @@
         <v>186</v>
       </c>
       <c r="X120" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="121" spans="1:24">
@@ -7168,7 +7168,7 @@
         <v>142</v>
       </c>
       <c r="T121" t="s">
-        <v>198</v>
+        <v>214</v>
       </c>
       <c r="U121" t="s">
         <v>123</v>
@@ -7180,7 +7180,7 @@
         <v>186</v>
       </c>
       <c r="X121" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="122" spans="1:24">
@@ -7227,7 +7227,7 @@
         <v>142</v>
       </c>
       <c r="T122" t="s">
-        <v>198</v>
+        <v>214</v>
       </c>
       <c r="U122" t="s">
         <v>123</v>
@@ -7239,7 +7239,7 @@
         <v>186</v>
       </c>
       <c r="X122" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="123" spans="1:24">
@@ -7289,7 +7289,7 @@
         <v>184</v>
       </c>
       <c r="T123" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U123" t="s">
         <v>120</v>
@@ -7298,7 +7298,7 @@
         <v>174</v>
       </c>
       <c r="X123" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="124" spans="1:24">
@@ -7348,7 +7348,7 @@
         <v>184</v>
       </c>
       <c r="T124" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U124" t="s">
         <v>120</v>
@@ -7357,7 +7357,7 @@
         <v>174</v>
       </c>
       <c r="X124" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="125" spans="1:24">
@@ -7407,7 +7407,7 @@
         <v>184</v>
       </c>
       <c r="T125" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U125" t="s">
         <v>120</v>
@@ -7416,7 +7416,7 @@
         <v>174</v>
       </c>
       <c r="X125" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="126" spans="1:24">
@@ -7466,7 +7466,7 @@
         <v>184</v>
       </c>
       <c r="T126" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U126" t="s">
         <v>120</v>
@@ -7475,7 +7475,7 @@
         <v>174</v>
       </c>
       <c r="X126" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="127" spans="1:24">
@@ -7525,7 +7525,7 @@
         <v>184</v>
       </c>
       <c r="T127" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U127" t="s">
         <v>120</v>
@@ -7534,7 +7534,7 @@
         <v>174</v>
       </c>
       <c r="X127" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="128" spans="1:24">
@@ -7584,7 +7584,7 @@
         <v>184</v>
       </c>
       <c r="T128" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U128" t="s">
         <v>120</v>
@@ -7593,7 +7593,7 @@
         <v>174</v>
       </c>
       <c r="X128" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="129" spans="1:24">
@@ -7643,7 +7643,7 @@
         <v>184</v>
       </c>
       <c r="T129" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U129" t="s">
         <v>120</v>
@@ -7652,7 +7652,7 @@
         <v>174</v>
       </c>
       <c r="X129" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="130" spans="1:24">
@@ -7702,7 +7702,7 @@
         <v>184</v>
       </c>
       <c r="T130" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U130" t="s">
         <v>120</v>
@@ -7711,7 +7711,7 @@
         <v>174</v>
       </c>
       <c r="X130" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="131" spans="1:24">
@@ -7761,7 +7761,7 @@
         <v>184</v>
       </c>
       <c r="T131" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U131" t="s">
         <v>120</v>
@@ -7770,7 +7770,7 @@
         <v>174</v>
       </c>
       <c r="X131" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="132" spans="1:24">
@@ -7820,7 +7820,7 @@
         <v>184</v>
       </c>
       <c r="T132" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U132" t="s">
         <v>120</v>
@@ -7829,7 +7829,7 @@
         <v>174</v>
       </c>
       <c r="X132" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="133" spans="1:24">
@@ -7879,7 +7879,7 @@
         <v>184</v>
       </c>
       <c r="T133" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U133" t="s">
         <v>120</v>
@@ -7888,7 +7888,7 @@
         <v>174</v>
       </c>
       <c r="X133" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="134" spans="1:24">
@@ -7938,7 +7938,7 @@
         <v>184</v>
       </c>
       <c r="T134" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U134" t="s">
         <v>120</v>
@@ -7947,7 +7947,7 @@
         <v>174</v>
       </c>
       <c r="X134" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="135" spans="1:24">
@@ -7994,7 +7994,7 @@
         <v>186</v>
       </c>
       <c r="T135" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="136" spans="1:24">
@@ -8041,7 +8041,7 @@
         <v>186</v>
       </c>
       <c r="T136" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="137" spans="1:24">
@@ -8088,7 +8088,7 @@
         <v>200</v>
       </c>
       <c r="T137" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="138" spans="1:24">
@@ -8135,7 +8135,7 @@
         <v>200</v>
       </c>
       <c r="T138" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="139" spans="1:24">
@@ -8182,7 +8182,7 @@
         <v>200</v>
       </c>
       <c r="T139" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="140" spans="1:24">
@@ -8229,7 +8229,7 @@
         <v>200</v>
       </c>
       <c r="T140" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="141" spans="1:24">
@@ -8724,7 +8724,7 @@
         <v>154</v>
       </c>
       <c r="T152" t="s">
-        <v>222</v>
+        <v>180</v>
       </c>
       <c r="U152" t="s">
         <v>127</v>
@@ -8783,7 +8783,7 @@
         <v>154</v>
       </c>
       <c r="T153" t="s">
-        <v>222</v>
+        <v>180</v>
       </c>
       <c r="U153" t="s">
         <v>127</v>
@@ -8842,7 +8842,7 @@
         <v>154</v>
       </c>
       <c r="T154" t="s">
-        <v>222</v>
+        <v>180</v>
       </c>
       <c r="U154" t="s">
         <v>127</v>
@@ -8901,7 +8901,7 @@
         <v>154</v>
       </c>
       <c r="T155" t="s">
-        <v>222</v>
+        <v>180</v>
       </c>
       <c r="U155" t="s">
         <v>127</v>
@@ -9406,7 +9406,7 @@
         <v>204</v>
       </c>
       <c r="T166" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="167" spans="1:24">
@@ -9453,7 +9453,7 @@
         <v>204</v>
       </c>
       <c r="T167" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="168" spans="1:24">
@@ -9767,16 +9767,16 @@
         <v>169</v>
       </c>
       <c r="T174" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="U174" t="s">
         <v>128</v>
       </c>
       <c r="V174" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="X174" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="175" spans="1:24">
@@ -9826,16 +9826,16 @@
         <v>169</v>
       </c>
       <c r="T175" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="U175" t="s">
         <v>128</v>
       </c>
       <c r="V175" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="X175" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="176" spans="1:24">
@@ -9885,16 +9885,16 @@
         <v>169</v>
       </c>
       <c r="T176" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="U176" t="s">
         <v>128</v>
       </c>
       <c r="V176" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="X176" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="177" spans="1:24">
@@ -9944,16 +9944,16 @@
         <v>169</v>
       </c>
       <c r="T177" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="U177" t="s">
         <v>128</v>
       </c>
       <c r="V177" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="X177" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="178" spans="1:24">
@@ -10006,10 +10006,10 @@
         <v>130</v>
       </c>
       <c r="V178" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="X178" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="179" spans="1:24">
@@ -10062,10 +10062,10 @@
         <v>130</v>
       </c>
       <c r="V179" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="X179" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="180" spans="1:24">
@@ -10118,10 +10118,10 @@
         <v>130</v>
       </c>
       <c r="V180" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="X180" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="181" spans="1:24">
@@ -10174,10 +10174,10 @@
         <v>130</v>
       </c>
       <c r="V181" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="X181" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="182" spans="1:24">
@@ -10534,7 +10534,7 @@
         <v>206</v>
       </c>
       <c r="T190" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="191" spans="1:24">
@@ -10669,7 +10669,7 @@
         <v>200</v>
       </c>
       <c r="T193" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="194" spans="1:24">
@@ -10716,7 +10716,7 @@
         <v>200</v>
       </c>
       <c r="T194" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="195" spans="1:24">
@@ -10763,7 +10763,7 @@
         <v>200</v>
       </c>
       <c r="T195" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="196" spans="1:24">
@@ -10810,7 +10810,7 @@
         <v>200</v>
       </c>
       <c r="T196" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="197" spans="1:24">
@@ -10995,7 +10995,7 @@
         <v>174</v>
       </c>
       <c r="X200" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="201" spans="1:24">
@@ -11048,7 +11048,7 @@
         <v>174</v>
       </c>
       <c r="X201" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="202" spans="1:24">
@@ -11101,7 +11101,7 @@
         <v>174</v>
       </c>
       <c r="X202" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="203" spans="1:24">
@@ -11154,7 +11154,7 @@
         <v>174</v>
       </c>
       <c r="X203" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="204" spans="1:24">
@@ -11201,7 +11201,7 @@
         <v>173</v>
       </c>
       <c r="T204" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="U204" t="s">
         <v>124</v>
@@ -11257,7 +11257,7 @@
         <v>173</v>
       </c>
       <c r="T205" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="U205" t="s">
         <v>124</v>
@@ -11313,7 +11313,7 @@
         <v>173</v>
       </c>
       <c r="T206" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="U206" t="s">
         <v>124</v>
@@ -11545,7 +11545,7 @@
         <v>174</v>
       </c>
       <c r="T211" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="212" spans="1:20">
@@ -11592,7 +11592,7 @@
         <v>174</v>
       </c>
       <c r="T212" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="213" spans="1:20">
@@ -11639,7 +11639,7 @@
         <v>174</v>
       </c>
       <c r="T213" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="214" spans="1:20">
@@ -11686,7 +11686,7 @@
         <v>174</v>
       </c>
       <c r="T214" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="215" spans="1:20">
@@ -11733,7 +11733,7 @@
         <v>173</v>
       </c>
       <c r="T215" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="216" spans="1:20">
@@ -12264,7 +12264,7 @@
         <v>208</v>
       </c>
       <c r="T227" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="228" spans="1:24">
@@ -12311,16 +12311,16 @@
         <v>169</v>
       </c>
       <c r="T228" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="U228" t="s">
         <v>128</v>
       </c>
       <c r="V228" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="X228" t="s">
-        <v>195</v>
+        <v>247</v>
       </c>
     </row>
     <row r="229" spans="1:24">
@@ -12367,16 +12367,16 @@
         <v>169</v>
       </c>
       <c r="T229" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="U229" t="s">
         <v>128</v>
       </c>
       <c r="V229" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="X229" t="s">
-        <v>195</v>
+        <v>247</v>
       </c>
     </row>
     <row r="230" spans="1:24">
@@ -12423,16 +12423,16 @@
         <v>169</v>
       </c>
       <c r="T230" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="U230" t="s">
         <v>128</v>
       </c>
       <c r="V230" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="X230" t="s">
-        <v>195</v>
+        <v>247</v>
       </c>
     </row>
     <row r="231" spans="1:24">
@@ -12479,16 +12479,16 @@
         <v>169</v>
       </c>
       <c r="T231" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="U231" t="s">
         <v>128</v>
       </c>
       <c r="V231" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="X231" t="s">
-        <v>195</v>
+        <v>247</v>
       </c>
     </row>
     <row r="232" spans="1:24">
@@ -12535,16 +12535,16 @@
         <v>169</v>
       </c>
       <c r="T232" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="U232" t="s">
         <v>128</v>
       </c>
       <c r="V232" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="X232" t="s">
-        <v>195</v>
+        <v>247</v>
       </c>
     </row>
     <row r="233" spans="1:24">
@@ -12591,16 +12591,16 @@
         <v>169</v>
       </c>
       <c r="T233" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="U233" t="s">
         <v>128</v>
       </c>
       <c r="V233" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="X233" t="s">
-        <v>195</v>
+        <v>247</v>
       </c>
     </row>
     <row r="234" spans="1:24">
@@ -12647,16 +12647,16 @@
         <v>169</v>
       </c>
       <c r="T234" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="U234" t="s">
         <v>128</v>
       </c>
       <c r="V234" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="X234" t="s">
-        <v>195</v>
+        <v>247</v>
       </c>
     </row>
     <row r="235" spans="1:24">
@@ -12703,16 +12703,16 @@
         <v>169</v>
       </c>
       <c r="T235" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="U235" t="s">
         <v>128</v>
       </c>
       <c r="V235" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="X235" t="s">
-        <v>195</v>
+        <v>247</v>
       </c>
     </row>
     <row r="236" spans="1:24">
@@ -12762,10 +12762,10 @@
         <v>131</v>
       </c>
       <c r="V236" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="W236" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="X236" t="s">
         <v>248</v>
@@ -12818,10 +12818,10 @@
         <v>131</v>
       </c>
       <c r="V237" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="W237" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="X237" t="s">
         <v>248</v>
@@ -12874,10 +12874,10 @@
         <v>131</v>
       </c>
       <c r="V238" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="W238" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="X238" t="s">
         <v>248</v>
@@ -13438,7 +13438,7 @@
         <v>208</v>
       </c>
       <c r="T250" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="251" spans="1:20">
@@ -13485,7 +13485,7 @@
         <v>201</v>
       </c>
       <c r="T251" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="252" spans="1:20">
@@ -13532,7 +13532,7 @@
         <v>201</v>
       </c>
       <c r="T252" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="253" spans="1:20">
@@ -13975,7 +13975,7 @@
         <v>184</v>
       </c>
       <c r="T262" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U262" t="s">
         <v>120</v>
@@ -13984,7 +13984,7 @@
         <v>174</v>
       </c>
       <c r="X262" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="263" spans="1:24">
@@ -14034,7 +14034,7 @@
         <v>184</v>
       </c>
       <c r="T263" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U263" t="s">
         <v>120</v>
@@ -14043,7 +14043,7 @@
         <v>174</v>
       </c>
       <c r="X263" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="264" spans="1:24">
@@ -14093,7 +14093,7 @@
         <v>184</v>
       </c>
       <c r="T264" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U264" t="s">
         <v>120</v>
@@ -14102,7 +14102,7 @@
         <v>174</v>
       </c>
       <c r="X264" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="265" spans="1:24">
@@ -14152,7 +14152,7 @@
         <v>184</v>
       </c>
       <c r="T265" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U265" t="s">
         <v>120</v>
@@ -14161,7 +14161,7 @@
         <v>174</v>
       </c>
       <c r="X265" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="266" spans="1:24">
@@ -14211,7 +14211,7 @@
         <v>184</v>
       </c>
       <c r="T266" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U266" t="s">
         <v>120</v>
@@ -14220,7 +14220,7 @@
         <v>174</v>
       </c>
       <c r="X266" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="267" spans="1:24">
@@ -14270,7 +14270,7 @@
         <v>184</v>
       </c>
       <c r="T267" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U267" t="s">
         <v>120</v>
@@ -14279,7 +14279,7 @@
         <v>174</v>
       </c>
       <c r="X267" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="268" spans="1:24">
@@ -14329,7 +14329,7 @@
         <v>184</v>
       </c>
       <c r="T268" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U268" t="s">
         <v>120</v>
@@ -14338,7 +14338,7 @@
         <v>174</v>
       </c>
       <c r="X268" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="269" spans="1:24">
@@ -14388,7 +14388,7 @@
         <v>184</v>
       </c>
       <c r="T269" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U269" t="s">
         <v>120</v>
@@ -14397,7 +14397,7 @@
         <v>174</v>
       </c>
       <c r="X269" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="270" spans="1:24">
@@ -14447,7 +14447,7 @@
         <v>184</v>
       </c>
       <c r="T270" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U270" t="s">
         <v>120</v>
@@ -14456,7 +14456,7 @@
         <v>174</v>
       </c>
       <c r="X270" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="271" spans="1:24">
@@ -14506,7 +14506,7 @@
         <v>184</v>
       </c>
       <c r="T271" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U271" t="s">
         <v>120</v>
@@ -14515,7 +14515,7 @@
         <v>174</v>
       </c>
       <c r="X271" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="272" spans="1:24">
@@ -14565,7 +14565,7 @@
         <v>184</v>
       </c>
       <c r="T272" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U272" t="s">
         <v>120</v>
@@ -14574,7 +14574,7 @@
         <v>174</v>
       </c>
       <c r="X272" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="273" spans="1:24">
@@ -14624,7 +14624,7 @@
         <v>184</v>
       </c>
       <c r="T273" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="U273" t="s">
         <v>120</v>
@@ -14633,7 +14633,7 @@
         <v>174</v>
       </c>
       <c r="X273" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="274" spans="1:24">
@@ -14680,16 +14680,16 @@
         <v>169</v>
       </c>
       <c r="T274" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="U274" t="s">
         <v>128</v>
       </c>
       <c r="V274" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="X274" t="s">
-        <v>195</v>
+        <v>247</v>
       </c>
     </row>
     <row r="275" spans="1:24">
@@ -14736,16 +14736,16 @@
         <v>169</v>
       </c>
       <c r="T275" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="U275" t="s">
         <v>128</v>
       </c>
       <c r="V275" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="X275" t="s">
-        <v>195</v>
+        <v>247</v>
       </c>
     </row>
     <row r="276" spans="1:24">
@@ -14792,16 +14792,16 @@
         <v>169</v>
       </c>
       <c r="T276" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="U276" t="s">
         <v>128</v>
       </c>
       <c r="V276" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="X276" t="s">
-        <v>195</v>
+        <v>247</v>
       </c>
     </row>
     <row r="277" spans="1:24">
@@ -14848,16 +14848,16 @@
         <v>169</v>
       </c>
       <c r="T277" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="U277" t="s">
         <v>128</v>
       </c>
       <c r="V277" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="X277" t="s">
-        <v>195</v>
+        <v>247</v>
       </c>
     </row>
     <row r="278" spans="1:24">
@@ -14904,16 +14904,16 @@
         <v>169</v>
       </c>
       <c r="T278" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="U278" t="s">
         <v>128</v>
       </c>
       <c r="V278" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="X278" t="s">
-        <v>195</v>
+        <v>247</v>
       </c>
     </row>
     <row r="279" spans="1:24">
@@ -14960,16 +14960,16 @@
         <v>169</v>
       </c>
       <c r="T279" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="U279" t="s">
         <v>128</v>
       </c>
       <c r="V279" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="X279" t="s">
-        <v>195</v>
+        <v>247</v>
       </c>
     </row>
     <row r="280" spans="1:24">
@@ -15016,16 +15016,16 @@
         <v>169</v>
       </c>
       <c r="T280" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="U280" t="s">
         <v>128</v>
       </c>
       <c r="V280" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="X280" t="s">
-        <v>195</v>
+        <v>247</v>
       </c>
     </row>
     <row r="281" spans="1:24">
@@ -15072,16 +15072,16 @@
         <v>169</v>
       </c>
       <c r="T281" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="U281" t="s">
         <v>128</v>
       </c>
       <c r="V281" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="X281" t="s">
-        <v>195</v>
+        <v>247</v>
       </c>
     </row>
     <row r="282" spans="1:24">
@@ -15131,7 +15131,7 @@
         <v>200</v>
       </c>
       <c r="T282" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="283" spans="1:24">
@@ -15181,7 +15181,7 @@
         <v>200</v>
       </c>
       <c r="T283" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="284" spans="1:24">
@@ -15231,7 +15231,7 @@
         <v>200</v>
       </c>
       <c r="T284" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="285" spans="1:24">
@@ -15281,7 +15281,7 @@
         <v>200</v>
       </c>
       <c r="T285" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="286" spans="1:24">

</xml_diff>